<commit_message>
Week 1 dataset curated: multilingual real audio + metadata
</commit_message>
<xml_diff>
--- a/metadata/aggregated_metadata.xlsx
+++ b/metadata/aggregated_metadata.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,969 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>filename</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>duration</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>accent</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>transcript</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>path</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>english_0.wav</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>The track appears on the compilation album "Kraftworks".</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>../datasets\english\english_0.wav</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>english_1.wav</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>The Massachusetts Division of Fisheries and Wildlife has stocked the Jones River with trout.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>../datasets\english\english_1.wav</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>english_2.wav</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>The most common playing format for poker tournaments is the "freezeout" format.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>../datasets\english\english_2.wav</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>english_3.wav</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Rafting became less important after the construction of the Murg Valley Railway.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>../datasets\english\english_3.wav</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>english_4.wav</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>My life is ridiculously tempestuous at times.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>../datasets\english\english_4.wav</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>spanish_0.wav</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>spanish</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>¿ Qué tal a tres de cinco ?</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>../datasets\spanish\spanish_0.wav</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>spanish_1.wav</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>spanish</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>vamos , quiero decir , que no soy de citas especiales .</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>../datasets\spanish\spanish_1.wav</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>spanish_2.wav</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>spanish</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>fray Lope , en aquel momento , colmaba otro vaso igual :</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>../datasets\spanish\spanish_2.wav</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>spanish_3.wav</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>spanish</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>hermanito . dice hermanito . anda ...</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>../datasets\spanish\spanish_3.wav</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>spanish_4.wav</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>spanish</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>tengo un mensaje para usted</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>../datasets\spanish\spanish_4.wav</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>mandarin_0.wav</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mandarin</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>性喜温暖润湿气候且耐寒。</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>../datasets\mandarin\mandarin_0.wav</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>mandarin_1.wav</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mandarin</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>不包括香山公园和八大处公园内部的景点。</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>../datasets\mandarin\mandarin_1.wav</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>mandarin_2.wav</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mandarin</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>汉代经济先后经历了繁荣和衰落两个极端的阶段。</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>../datasets\mandarin\mandarin_2.wav</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>mandarin_3.wav</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mandarin</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>后来在今中山五路与北京路交界处出现夜间花市。</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>../datasets\mandarin\mandarin_3.wav</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>mandarin_4.wav</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mandarin</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>外套则以黑色为主。</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>../datasets\mandarin\mandarin_4.wav</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>french_0.wav</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>french</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Il est dissous à Trèves.</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>../datasets\french\french_0.wav</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>french_1.wav</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>french</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Les candidats sont présentés par le Fili.</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>../datasets\french\french_1.wav</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>french_2.wav</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>french</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Il y rencontre plusieurs éditeurs dont il rejette pourtant les propositions de traductions.</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>../datasets\french\french_2.wav</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>french_3.wav</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>french</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Le duo s'associe et collabore jusqu'à la mort de Dolan.</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>../datasets\french\french_3.wav</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>french_4.wav</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>french</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Il représente le de Californie qui englobe l'ouest du comté de Riverside.</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>../datasets\french\french_4.wav</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>german_0.wav</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>german</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Deutschland Deutsch</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Wo ist denn die Fernbedienung?</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>../datasets\german\german_0.wav</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>german_1.wav</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>german</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Deutschland Deutsch</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Haben Sie zollpflichtige Ware dabei?</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>../datasets\german\german_1.wav</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>german_2.wav</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>german</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Deutschland Deutsch</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Was heißt das auf Albanisch?</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>../datasets\german\german_2.wav</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>german_3.wav</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>german</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Ich fürchte sehr, dass das System der Ratspräsidentschaft diese durcheinander bringen wird.</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>../datasets\german\german_3.wav</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>german_4.wav</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>german</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Die Management-Pläne für die Generaldirektionen haben sich verbessert.</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>../datasets\german\german_4.wav</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>CommonVoice</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>